<commit_message>
Separate lastname for sortability
</commit_message>
<xml_diff>
--- a/data/view/attendance/flag.xlsx
+++ b/data/view/attendance/flag.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20055" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="132" windowWidth="20052" windowHeight="7956"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -14,12 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>No.</t>
-  </si>
-  <si>
-    <t>Name</t>
   </si>
   <si>
     <t>Sex</t>
@@ -29,6 +26,12 @@
   </si>
   <si>
     <t>Time</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
   </si>
 </sst>
 </file>
@@ -133,9 +136,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -152,6 +152,9 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -447,80 +450,86 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32" style="1" customWidth="1"/>
-    <col min="3" max="3" width="4.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1"/>
-    <col min="6" max="6" width="9.140625" style="3"/>
-    <col min="7" max="7" width="9.140625" style="1"/>
-    <col min="8" max="8" width="9.140625" style="3"/>
-    <col min="9" max="9" width="9.140625" style="1"/>
-    <col min="10" max="10" width="9.140625" style="3"/>
-    <col min="11" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="4.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.21875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="4.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="1"/>
+    <col min="7" max="7" width="9.109375" style="3"/>
+    <col min="8" max="8" width="9.109375" style="1"/>
+    <col min="9" max="9" width="9.109375" style="3"/>
+    <col min="10" max="10" width="9.109375" style="1"/>
+    <col min="11" max="11" width="9.109375" style="3"/>
+    <col min="12" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:12" ht="21">
+      <c r="A1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+    </row>
+    <row r="2" spans="1:12" ht="21.75" customHeight="1">
+      <c r="A2" s="10">
+        <v>44562</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-    </row>
-    <row r="2" spans="1:11" ht="21.75" customHeight="1">
-      <c r="A2" s="11">
-        <v>44562</v>
-      </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-    </row>
-    <row r="3" spans="1:11" ht="15">
-      <c r="A3" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="7"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>